<commit_message>
fix notif and download strakom
</commit_message>
<xml_diff>
--- a/uploads/strakom_unggulan.xlsx
+++ b/uploads/strakom_unggulan.xlsx
@@ -448,7 +448,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -645,126 +645,6 @@
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>testing program unggulan daerah 120623</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>222222</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>222222</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>222222</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>testing program unggulan daerah 120623</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>222222</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>222222</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>2222222</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD 130624</t>
-        </is>
-      </c>
-      <c r="C10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD</t>
-        </is>
-      </c>
-      <c r="D10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD</t>
-        </is>
-      </c>
-      <c r="E10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD</t>
-        </is>
-      </c>
-      <c r="F10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD</t>
-        </is>
-      </c>
-      <c r="G10" s="0" t="inlineStr">
-        <is>
-          <t>test KSD</t>
-        </is>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="0" t="inlineStr">
-        <is>
-          <t>ssssss</t>
-        </is>
-      </c>
-      <c r="C11" s="0" t="inlineStr">
-        <is>
-          <t>sssssss</t>
-        </is>
-      </c>
-      <c r="D11" s="0" t="inlineStr">
-        <is>
-          <t>ssssssfff</t>
-        </is>
-      </c>
-      <c r="E11" s="0" t="inlineStr">
-        <is>
-          <t>ssssssff</t>
-        </is>
-      </c>
-      <c r="F11" s="0" t="inlineStr">
-        <is>
-          <t>sssssfff</t>
-        </is>
-      </c>
-      <c r="G11" s="0" t="inlineStr">
-        <is>
-          <t>sssssffff</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>

</xml_diff>